<commit_message>
problem a | b
</commit_message>
<xml_diff>
--- a/problem_a/generated.xlsx
+++ b/problem_a/generated.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burse\Documents\Projects\Hashcode\Pizza-\problem_a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B60BE583-B472-41CD-89E7-7170AED6761D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EA127B-51AE-4655-8786-AA17689ED544}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="213"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="213" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generated" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="23">
   <si>
     <t>method</t>
   </si>
@@ -78,12 +78,30 @@
   <si>
     <t>parent_method</t>
   </si>
+  <si>
+    <t>onion pepper olive at the top</t>
+  </si>
+  <si>
+    <t>chicken basil at the top</t>
+  </si>
+  <si>
+    <t>tomato mushroom basil at the top</t>
+  </si>
+  <si>
+    <t>chicken mushroom pepper at the top</t>
+  </si>
+  <si>
+    <t>mushroom tomato basil at the top</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000000000000000"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,8 +245,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,6 +442,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,11 +688,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -674,6 +712,20 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1028,153 +1080,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AM37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.26953125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="2.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.90625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="2.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.88671875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="5" style="2" customWidth="1"/>
-    <col min="25" max="25" width="2.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.7265625" style="2" customWidth="1"/>
-    <col min="33" max="33" width="2.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.6640625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="5" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="8.7265625" style="1"/>
+    <col min="41" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-      <c r="I1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="I1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="7"/>
+      <c r="Q1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="6"/>
-      <c r="Y1" s="4" t="s">
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="7"/>
+      <c r="Y1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
-      <c r="AG1" s="4" t="s">
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="7"/>
+      <c r="AG1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="7"/>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="I2" s="7" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="9"/>
-      <c r="Q2" s="4" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="10"/>
+      <c r="Q2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="6"/>
-      <c r="Y2" s="4" t="s">
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="7"/>
+      <c r="Y2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="6"/>
-      <c r="AG2" s="4" t="s">
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="7"/>
+      <c r="AG2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="7"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,7 +1318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1336,7 +1388,7 @@
       <c r="Z4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AA4" s="4">
         <v>0.26</v>
       </c>
       <c r="AB4" s="1">
@@ -1357,7 +1409,7 @@
       <c r="AH4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AI4" s="4">
         <v>0.27</v>
       </c>
       <c r="AJ4" s="1">
@@ -1373,14 +1425,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>0</v>
       </c>
       <c r="D5" s="1">
@@ -1401,7 +1453,7 @@
       <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="4">
         <v>0.01</v>
       </c>
       <c r="L5" s="1">
@@ -1422,7 +1474,7 @@
       <c r="R5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="4">
         <v>0.01</v>
       </c>
       <c r="T5" s="1">
@@ -1480,14 +1532,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>0.27</v>
       </c>
       <c r="D6" s="1">
@@ -1508,7 +1560,7 @@
       <c r="J6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="4">
         <v>0.26</v>
       </c>
       <c r="L6" s="1">
@@ -1529,7 +1581,7 @@
       <c r="R6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="4">
         <v>0.26</v>
       </c>
       <c r="T6" s="1">
@@ -1587,7 +1639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1657,7 +1709,7 @@
       <c r="Z7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AA7" s="4">
         <v>0.03</v>
       </c>
       <c r="AB7" s="1">
@@ -1678,7 +1730,7 @@
       <c r="AH7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AI7" s="3">
+      <c r="AI7" s="4">
         <v>0.01</v>
       </c>
       <c r="AJ7" s="1">
@@ -1694,14 +1746,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>0.27</v>
       </c>
       <c r="D8" s="1">
@@ -1785,7 +1837,7 @@
       <c r="AH8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AI8" s="3">
+      <c r="AI8" s="4">
         <v>0.26</v>
       </c>
       <c r="AJ8" s="1">
@@ -1801,7 +1853,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1829,7 +1881,7 @@
       <c r="J9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="4">
         <v>0</v>
       </c>
       <c r="L9" s="1">
@@ -1850,7 +1902,7 @@
       <c r="R9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="4">
         <v>0.01</v>
       </c>
       <c r="T9" s="1">
@@ -1871,7 +1923,7 @@
       <c r="Z9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AA9" s="3">
+      <c r="AA9" s="4">
         <v>0.03</v>
       </c>
       <c r="AB9" s="1">
@@ -1908,7 +1960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1936,7 +1988,7 @@
       <c r="J10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="4">
         <v>0.27</v>
       </c>
       <c r="L10" s="1">
@@ -1957,7 +2009,7 @@
       <c r="R10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10" s="4">
         <v>0.26</v>
       </c>
       <c r="T10" s="1">
@@ -1978,7 +2030,7 @@
       <c r="Z10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AA10" s="3">
+      <c r="AA10" s="4">
         <v>0.26</v>
       </c>
       <c r="AB10" s="1">
@@ -2015,14 +2067,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>0.01</v>
       </c>
       <c r="D11" s="1">
@@ -2106,7 +2158,7 @@
       <c r="AH11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AI11" s="3">
+      <c r="AI11" s="4">
         <v>0</v>
       </c>
       <c r="AJ11" s="1">
@@ -2122,14 +2174,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>0.26</v>
       </c>
       <c r="D12" s="1">
@@ -2150,7 +2202,7 @@
       <c r="J12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="4">
         <v>0.27</v>
       </c>
       <c r="L12" s="1">
@@ -2171,7 +2223,7 @@
       <c r="R12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S12" s="3">
+      <c r="S12" s="4">
         <v>0.26</v>
       </c>
       <c r="T12" s="1">
@@ -2192,7 +2244,7 @@
       <c r="Z12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AA12" s="3">
+      <c r="AA12" s="4">
         <v>0.26</v>
       </c>
       <c r="AB12" s="1">
@@ -2213,7 +2265,7 @@
       <c r="AH12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AI12" s="3">
+      <c r="AI12" s="4">
         <v>0.27</v>
       </c>
       <c r="AJ12" s="1">
@@ -2229,7 +2281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -2336,7 +2388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -2443,14 +2495,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>0.01</v>
       </c>
       <c r="D15" s="1">
@@ -2471,7 +2523,7 @@
       <c r="J15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="4">
         <v>0.01</v>
       </c>
       <c r="L15" s="1">
@@ -2492,7 +2544,7 @@
       <c r="R15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S15" s="3">
+      <c r="S15" s="4">
         <v>0.01</v>
       </c>
       <c r="T15" s="1">
@@ -2513,7 +2565,7 @@
       <c r="Z15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AA15" s="3">
+      <c r="AA15" s="4">
         <v>0</v>
       </c>
       <c r="AB15" s="1">
@@ -2534,7 +2586,7 @@
       <c r="AH15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AI15" s="3">
+      <c r="AI15" s="4">
         <v>0</v>
       </c>
       <c r="AJ15" s="1">
@@ -2550,7 +2602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -2657,7 +2709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -2764,8 +2816,1727 @@
         <v>6</v>
       </c>
     </row>
+    <row r="19" spans="1:39" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12">
+        <v>0.26</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="J19" s="12">
+        <v>0.23999999999999899</v>
+      </c>
+      <c r="P19" s="13"/>
+      <c r="R19" s="12">
+        <v>0.26</v>
+      </c>
+      <c r="X19" s="13"/>
+      <c r="Z19" s="12">
+        <v>0.20999999999999899</v>
+      </c>
+      <c r="AF19" s="13"/>
+      <c r="AH19" s="12">
+        <v>0.22999999999999901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="7"/>
+      <c r="Q20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="7"/>
+      <c r="Y20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="7"/>
+      <c r="AG20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
+      <c r="AK20" s="6"/>
+      <c r="AL20" s="6"/>
+      <c r="AM20" s="7"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>2</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="T22" s="1">
+        <v>0</v>
+      </c>
+      <c r="U22" s="1">
+        <v>2</v>
+      </c>
+      <c r="V22" s="1">
+        <v>1</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI22" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="AJ22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>2</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>2</v>
+      </c>
+      <c r="V23" s="1">
+        <v>1</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI23" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AJ23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.21</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1">
+        <v>3</v>
+      </c>
+      <c r="N24" s="1">
+        <v>2</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>2</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="T24" s="1">
+        <v>1</v>
+      </c>
+      <c r="U24" s="1">
+        <v>3</v>
+      </c>
+      <c r="V24" s="1">
+        <v>2</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG24" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI24" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AJ24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL24" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>3</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>3</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="T25" s="1">
+        <v>1</v>
+      </c>
+      <c r="U25" s="1">
+        <v>3</v>
+      </c>
+      <c r="V25" s="1">
+        <v>2</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI25" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="AJ25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL25" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.21</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="1">
+        <v>4</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>3</v>
+      </c>
+      <c r="N26" s="1">
+        <v>2</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>4</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S26" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="T26" s="1">
+        <v>1</v>
+      </c>
+      <c r="U26" s="1">
+        <v>3</v>
+      </c>
+      <c r="V26" s="1">
+        <v>2</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG26" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI26" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AJ26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL26" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I27" s="1">
+        <v>5</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1">
+        <v>3</v>
+      </c>
+      <c r="N27" s="1">
+        <v>2</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>5</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S27" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="T27" s="1">
+        <v>1</v>
+      </c>
+      <c r="U27" s="1">
+        <v>3</v>
+      </c>
+      <c r="V27" s="1">
+        <v>2</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG27" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI27" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="AJ27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL27" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="1">
+        <v>6</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="L28" s="1">
+        <v>2</v>
+      </c>
+      <c r="M28" s="1">
+        <v>4</v>
+      </c>
+      <c r="N28" s="1">
+        <v>3</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>6</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="T28" s="1">
+        <v>2</v>
+      </c>
+      <c r="U28" s="1">
+        <v>4</v>
+      </c>
+      <c r="V28" s="1">
+        <v>3</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG28" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI28" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="AJ28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL28" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.04</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>4</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="1">
+        <v>7</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2</v>
+      </c>
+      <c r="M29" s="1">
+        <v>4</v>
+      </c>
+      <c r="N29" s="1">
+        <v>3</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>7</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="T29" s="1">
+        <v>2</v>
+      </c>
+      <c r="U29" s="1">
+        <v>4</v>
+      </c>
+      <c r="V29" s="1">
+        <v>3</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD29" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG29" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI29" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AJ29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL29" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM29" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="1">
+        <v>8</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="L30" s="1">
+        <v>2</v>
+      </c>
+      <c r="M30" s="1">
+        <v>4</v>
+      </c>
+      <c r="N30" s="1">
+        <v>3</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>8</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="T30" s="1">
+        <v>2</v>
+      </c>
+      <c r="U30" s="1">
+        <v>4</v>
+      </c>
+      <c r="V30" s="1">
+        <v>3</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC30" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD30" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG30" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI30" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="AJ30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL30" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="1">
+        <v>9</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="L31" s="1">
+        <v>2</v>
+      </c>
+      <c r="M31" s="1">
+        <v>4</v>
+      </c>
+      <c r="N31" s="1">
+        <v>3</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>9</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S31" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="T31" s="1">
+        <v>2</v>
+      </c>
+      <c r="U31" s="1">
+        <v>4</v>
+      </c>
+      <c r="V31" s="1">
+        <v>3</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC31" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD31" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG31" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI31" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AJ31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL31" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>5</v>
+      </c>
+      <c r="F32" s="1">
+        <v>4</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="1">
+        <v>10</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L32" s="1">
+        <v>3</v>
+      </c>
+      <c r="M32" s="1">
+        <v>5</v>
+      </c>
+      <c r="N32" s="1">
+        <v>4</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>10</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S32" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="T32" s="1">
+        <v>0</v>
+      </c>
+      <c r="U32" s="1">
+        <v>5</v>
+      </c>
+      <c r="V32" s="1">
+        <v>4</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG32" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI32" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AJ32" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK32" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL32" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>5</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="1">
+        <v>11</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="L33" s="1">
+        <v>3</v>
+      </c>
+      <c r="M33" s="1">
+        <v>5</v>
+      </c>
+      <c r="N33" s="1">
+        <v>4</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>11</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="T33" s="1">
+        <v>0</v>
+      </c>
+      <c r="U33" s="1">
+        <v>5</v>
+      </c>
+      <c r="V33" s="1">
+        <v>4</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG33" s="1">
+        <v>11</v>
+      </c>
+      <c r="AH33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI33" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AJ33" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK33" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL33" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>5</v>
+      </c>
+      <c r="F34" s="1">
+        <v>4</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="1">
+        <v>12</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L34" s="1">
+        <v>3</v>
+      </c>
+      <c r="M34" s="1">
+        <v>5</v>
+      </c>
+      <c r="N34" s="1">
+        <v>4</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>12</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0</v>
+      </c>
+      <c r="U34" s="1">
+        <v>5</v>
+      </c>
+      <c r="V34" s="1">
+        <v>4</v>
+      </c>
+      <c r="W34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>12</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA34" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC34" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD34" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG34" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI34" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AJ34" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK34" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL34" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>5</v>
+      </c>
+      <c r="F35" s="1">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="1">
+        <v>13</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="L35" s="1">
+        <v>3</v>
+      </c>
+      <c r="M35" s="1">
+        <v>5</v>
+      </c>
+      <c r="N35" s="1">
+        <v>4</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>13</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1">
+        <v>5</v>
+      </c>
+      <c r="V35" s="1">
+        <v>4</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>13</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG35" s="1">
+        <v>13</v>
+      </c>
+      <c r="AH35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI35" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AJ35" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK35" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL35" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" s="18" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A37" s="14">
+        <v>0</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="14">
+        <v>1</v>
+      </c>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="14">
+        <v>2</v>
+      </c>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="17"/>
+      <c r="Y37" s="14">
+        <v>3</v>
+      </c>
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="15"/>
+      <c r="AD37" s="15"/>
+      <c r="AE37" s="16"/>
+      <c r="AF37" s="17"/>
+      <c r="AG37" s="14">
+        <v>4</v>
+      </c>
+      <c r="AH37" s="15"/>
+      <c r="AI37" s="15"/>
+      <c r="AJ37" s="15"/>
+      <c r="AK37" s="15"/>
+      <c r="AL37" s="15"/>
+      <c r="AM37" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="20">
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="Y37:AE37"/>
+    <mergeCell ref="Q37:W37"/>
+    <mergeCell ref="I37:O37"/>
+    <mergeCell ref="AG37:AM37"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="I20:O20"/>
+    <mergeCell ref="Q20:W20"/>
+    <mergeCell ref="Y20:AE20"/>
+    <mergeCell ref="AG20:AM20"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="Q1:W1"/>
@@ -2778,5 +4549,6 @@
     <mergeCell ref="AG2:AM2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>